<commit_message>
Page Object With Factories
</commit_message>
<xml_diff>
--- a/PageObjectFactories/src/test/resources/com/pol/excel/TestData.xlsx
+++ b/PageObjectFactories/src/test/resources/com/pol/excel/TestData.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7950" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="20055" windowHeight="7950" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
     <sheet name="LoginTest" sheetId="1" r:id="rId2"/>
-    <sheet name="CreateAccountTest" sheetId="4" r:id="rId3"/>
+    <sheet name="FlightSearchTest" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="15">
   <si>
     <t>TCID</t>
   </si>
@@ -27,9 +27,6 @@
     <t>Y</t>
   </si>
   <si>
-    <t>RunMode</t>
-  </si>
-  <si>
     <t>LoginTest</t>
   </si>
   <si>
@@ -49,19 +46,41 @@
   </si>
   <si>
     <t>sel1</t>
+  </si>
+  <si>
+    <t>FlightSearchTest</t>
+  </si>
+  <si>
+    <t>ram@gmail.com</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Hr@gail.com</t>
+  </si>
+  <si>
+    <t>runmode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -81,13 +100,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -380,10 +405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -401,9 +426,17 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -414,10 +447,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -428,27 +461,53 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
         <v>5</v>
       </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
       <c r="C1" t="s">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
+        <v>12</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A3" r:id="rId1"/>
+    <hyperlink ref="A4" r:id="rId2"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -457,8 +516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -468,12 +527,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>